<commit_message>
minor changes to Fantasy setup
</commit_message>
<xml_diff>
--- a/data/2024/FantasySkiLeagueResults_Aggregated.xlsx
+++ b/data/2024/FantasySkiLeagueResults_Aggregated.xlsx
@@ -48,12 +48,12 @@
     <t xml:space="preserve">Topshelf </t>
   </si>
   <si>
+    <t>Suzanne's Quick Finishers</t>
+  </si>
+  <si>
     <t>All Fun little Glory</t>
   </si>
   <si>
-    <t>Suzanne's Quick Finishers</t>
-  </si>
-  <si>
     <t xml:space="preserve">Will's RealGudPros </t>
   </si>
   <si>
@@ -162,46 +162,46 @@
     <t>Jocelyn French</t>
   </si>
   <si>
+    <t>Sean Cotnam</t>
+  </si>
+  <si>
+    <t>Joanna Perrault</t>
+  </si>
+  <si>
+    <t>Rob Reid</t>
+  </si>
+  <si>
+    <t>Earl Duffy</t>
+  </si>
+  <si>
+    <t>Troy Harrison</t>
+  </si>
+  <si>
+    <t>Linda Leistner</t>
+  </si>
+  <si>
+    <t>Tushar Mehta</t>
+  </si>
+  <si>
+    <t>Mark Sandell</t>
+  </si>
+  <si>
+    <t>Tori Abbott</t>
+  </si>
+  <si>
+    <t>Audun Bredur</t>
+  </si>
+  <si>
+    <t>Will Stewart</t>
+  </si>
+  <si>
+    <t>Peter Daly</t>
+  </si>
+  <si>
+    <t>Peter Moorhead</t>
+  </si>
+  <si>
     <t>Brad Brock</t>
-  </si>
-  <si>
-    <t>Joanna Perrault</t>
-  </si>
-  <si>
-    <t>Rob Reid</t>
-  </si>
-  <si>
-    <t>Earl Duffy</t>
-  </si>
-  <si>
-    <t>Troy Harrison</t>
-  </si>
-  <si>
-    <t>Linda Leistner</t>
-  </si>
-  <si>
-    <t>Tushar Mehta</t>
-  </si>
-  <si>
-    <t>Mark Sandell</t>
-  </si>
-  <si>
-    <t>Sean Cotnam</t>
-  </si>
-  <si>
-    <t>Tori Abbott</t>
-  </si>
-  <si>
-    <t>Audun Bredur</t>
-  </si>
-  <si>
-    <t>Will Stewart</t>
-  </si>
-  <si>
-    <t>Peter Daly</t>
-  </si>
-  <si>
-    <t>Peter Moorhead</t>
   </si>
   <si>
     <t>Erica Reid</t>
@@ -639,7 +639,7 @@
         <v>7</v>
       </c>
       <c r="B7">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="8" spans="1:2">
@@ -743,7 +743,7 @@
     </row>
     <row r="3" spans="1:3">
       <c r="A3" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B3">
         <v>2</v>
@@ -754,7 +754,7 @@
     </row>
     <row r="4" spans="1:3">
       <c r="A4" t="s">
-        <v>44</v>
+        <v>57</v>
       </c>
       <c r="B4">
         <v>8</v>
@@ -855,7 +855,7 @@
     </row>
     <row r="2" spans="1:3">
       <c r="A2" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B2">
         <v>8</v>
@@ -1000,7 +1000,7 @@
     </row>
     <row r="4" spans="1:3">
       <c r="A4" t="s">
-        <v>52</v>
+        <v>44</v>
       </c>
       <c r="B4">
         <v>5</v>
@@ -1123,7 +1123,7 @@
     </row>
     <row r="4" spans="1:3">
       <c r="A4" t="s">
-        <v>52</v>
+        <v>44</v>
       </c>
       <c r="B4">
         <v>5</v>
@@ -1347,7 +1347,7 @@
     </row>
     <row r="2" spans="1:3">
       <c r="A2" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B2">
         <v>8</v>
@@ -1987,10 +1987,10 @@
         <v>44</v>
       </c>
       <c r="B4">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="C4">
-        <v>4</v>
+        <v>6</v>
       </c>
     </row>
     <row r="5" spans="1:3">
@@ -2230,7 +2230,7 @@
     </row>
     <row r="4" spans="1:3">
       <c r="A4" t="s">
-        <v>52</v>
+        <v>44</v>
       </c>
       <c r="B4">
         <v>5</v>
@@ -2263,7 +2263,7 @@
     </row>
     <row r="7" spans="1:3">
       <c r="A7" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B7">
         <v>2</v>
@@ -2285,7 +2285,7 @@
     </row>
     <row r="9" spans="1:3">
       <c r="A9" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B9">
         <v>7</v>
@@ -2331,7 +2331,7 @@
     </row>
     <row r="2" spans="1:3">
       <c r="A2" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B2">
         <v>8</v>
@@ -2364,7 +2364,7 @@
     </row>
     <row r="5" spans="1:3">
       <c r="A5" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B5">
         <v>4</v>

</xml_diff>